<commit_message>
combine input and output sankey
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smn\Repos\Sankey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4527C59E-4B0E-4AA0-A18C-4935C724E90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5547E677-7394-41A0-B0D7-878215922CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54600" yWindow="-5595" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54600" yWindow="-5595" windowWidth="25800" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="expenses" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Cat 1</t>
   </si>
@@ -64,13 +64,19 @@
     <t>Job</t>
   </si>
   <si>
-    <t>Erbe</t>
-  </si>
-  <si>
     <t>Novatec</t>
   </si>
   <si>
     <t>Vodafone</t>
+  </si>
+  <si>
+    <t>gehalt</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -390,13 +396,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -466,7 +473,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -481,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A418038-3858-44F3-9037-808E24BD9285}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,10 +516,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -522,14 +529,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>90</v>

</xml_diff>